<commit_message>
Update 28 Maret 2020
</commit_message>
<xml_diff>
--- a/Daerah Istimewa Yogyakarta/01_DIY_Rekapitulasi_24032020.xlsx
+++ b/Daerah Istimewa Yogyakarta/01_DIY_Rekapitulasi_24032020.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>REKAPITULASI HARIAN KASUS COVID-19</t>
   </si>
@@ -40,6 +40,9 @@
     <t>Menunggu Hasil Lab</t>
   </si>
   <si>
+    <t>PDP</t>
+  </si>
+  <si>
     <t>13/3/2020</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
   </si>
   <si>
     <t>27/3/2020</t>
+  </si>
+  <si>
+    <t>28/3/2020</t>
   </si>
 </sst>
 </file>
@@ -117,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border/>
     <border>
       <left style="thin">
@@ -159,6 +165,14 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
     </border>
     <border>
       <left style="thin">
@@ -189,38 +203,37 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -510,8 +523,8 @@
     <col customWidth="1" min="1" max="1" width="13.57"/>
     <col customWidth="1" min="2" max="5" width="8.71"/>
     <col customWidth="1" min="6" max="6" width="12.43"/>
-    <col customWidth="1" min="7" max="7" width="13.14"/>
-    <col customWidth="1" min="8" max="11" width="8.71"/>
+    <col customWidth="1" min="7" max="8" width="13.14"/>
+    <col customWidth="1" min="9" max="9" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -530,89 +543,85 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="7"/>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="11">
         <v>44077.0</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="10">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="11">
         <v>44107.0</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="10">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="11">
         <v>44138.0</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="10">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="11">
         <v>44168.0</v>
-      </c>
-      <c r="B7" s="12">
-        <v>13.0</v>
-      </c>
-      <c r="C7" s="12">
-        <v>11.0</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="G7" s="12">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="12" t="s">
-        <v>9</v>
       </c>
       <c r="B8" s="12">
         <v>13.0</v>
@@ -630,6 +639,9 @@
         <v>0.0</v>
       </c>
       <c r="G8" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="H8" s="12">
         <v>2.0</v>
       </c>
     </row>
@@ -638,10 +650,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="12">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="C9" s="12">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="D9" s="12">
         <v>0.0</v>
@@ -653,6 +665,9 @@
         <v>0.0</v>
       </c>
       <c r="G9" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="12">
         <v>2.0</v>
       </c>
     </row>
@@ -661,13 +676,13 @@
         <v>11</v>
       </c>
       <c r="B10" s="12">
-        <v>17.0</v>
+        <v>14.0</v>
       </c>
       <c r="C10" s="12">
         <v>12.0</v>
       </c>
       <c r="D10" s="12">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E10" s="12">
         <v>0.0</v>
@@ -676,7 +691,10 @@
         <v>0.0</v>
       </c>
       <c r="G10" s="12">
-        <v>4.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="H10" s="12">
+        <v>2.0</v>
       </c>
     </row>
     <row r="11">
@@ -684,7 +702,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="12">
-        <v>22.0</v>
+        <v>17.0</v>
       </c>
       <c r="C11" s="12">
         <v>12.0</v>
@@ -699,7 +717,10 @@
         <v>0.0</v>
       </c>
       <c r="G11" s="12">
-        <v>9.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="H11" s="12">
+        <v>4.0</v>
       </c>
     </row>
     <row r="12">
@@ -707,10 +728,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="12">
-        <v>24.0</v>
+        <v>22.0</v>
       </c>
       <c r="C12" s="12">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
       <c r="D12" s="12">
         <v>1.0</v>
@@ -722,6 +743,9 @@
         <v>0.0</v>
       </c>
       <c r="G12" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="H12" s="12">
         <v>9.0</v>
       </c>
     </row>
@@ -730,13 +754,13 @@
         <v>14</v>
       </c>
       <c r="B13" s="12">
-        <v>31.0</v>
+        <v>24.0</v>
       </c>
       <c r="C13" s="12">
         <v>14.0</v>
       </c>
       <c r="D13" s="12">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E13" s="12">
         <v>0.0</v>
@@ -745,7 +769,10 @@
         <v>0.0</v>
       </c>
       <c r="G13" s="12">
-        <v>15.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="H13" s="12">
+        <v>9.0</v>
       </c>
     </row>
     <row r="14">
@@ -753,22 +780,25 @@
         <v>15</v>
       </c>
       <c r="B14" s="12">
-        <v>37.0</v>
+        <v>31.0</v>
       </c>
       <c r="C14" s="12">
+        <v>14.0</v>
+      </c>
+      <c r="D14" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="H14" s="12">
         <v>15.0</v>
-      </c>
-      <c r="D14" s="12">
-        <v>4.0</v>
-      </c>
-      <c r="E14" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="F14" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="G14" s="12">
-        <v>18.0</v>
       </c>
     </row>
     <row r="15">
@@ -776,22 +806,25 @@
         <v>16</v>
       </c>
       <c r="B15" s="12">
-        <v>56.0</v>
+        <v>37.0</v>
       </c>
       <c r="C15" s="12">
-        <v>18.0</v>
+        <v>15.0</v>
       </c>
       <c r="D15" s="12">
         <v>4.0</v>
       </c>
       <c r="E15" s="12">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F15" s="12">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G15" s="12">
-        <v>34.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="H15" s="12">
+        <v>18.0</v>
       </c>
     </row>
     <row r="16">
@@ -799,22 +832,25 @@
         <v>17</v>
       </c>
       <c r="B16" s="12">
-        <v>71.0</v>
+        <v>56.0</v>
       </c>
       <c r="C16" s="12">
         <v>18.0</v>
       </c>
       <c r="D16" s="12">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="E16" s="12">
         <v>1.0</v>
       </c>
       <c r="F16" s="12">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G16" s="12">
-        <v>48.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="H16" s="12">
+        <v>34.0</v>
       </c>
     </row>
     <row r="17">
@@ -822,10 +858,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="12">
-        <v>76.0</v>
+        <v>71.0</v>
       </c>
       <c r="C17" s="12">
-        <v>20.0</v>
+        <v>18.0</v>
       </c>
       <c r="D17" s="12">
         <v>5.0</v>
@@ -834,10 +870,13 @@
         <v>1.0</v>
       </c>
       <c r="F17" s="12">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="G17" s="12">
-        <v>51.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="H17" s="12">
+        <v>48.0</v>
       </c>
     </row>
     <row r="18">
@@ -845,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="12">
-        <v>86.0</v>
+        <v>76.0</v>
       </c>
       <c r="C18" s="12">
         <v>20.0</v>
@@ -857,10 +896,13 @@
         <v>1.0</v>
       </c>
       <c r="F18" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="G18" s="12">
         <v>2.0</v>
       </c>
-      <c r="G18" s="12">
-        <v>61.0</v>
+      <c r="H18" s="12">
+        <v>51.0</v>
       </c>
     </row>
     <row r="19">
@@ -868,22 +910,25 @@
         <v>20</v>
       </c>
       <c r="B19" s="12">
-        <v>98.0</v>
+        <v>86.0</v>
       </c>
       <c r="C19" s="12">
-        <v>30.0</v>
+        <v>20.0</v>
       </c>
       <c r="D19" s="12">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="E19" s="12">
         <v>1.0</v>
       </c>
       <c r="F19" s="12">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="G19" s="12">
-        <v>62.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="H19" s="12">
+        <v>61.0</v>
       </c>
     </row>
     <row r="20">
@@ -891,22 +936,25 @@
         <v>21</v>
       </c>
       <c r="B20" s="12">
-        <v>115.0</v>
+        <v>98.0</v>
       </c>
       <c r="C20" s="12">
-        <v>33.0</v>
+        <v>30.0</v>
       </c>
       <c r="D20" s="12">
-        <v>18.0</v>
+        <v>6.0</v>
       </c>
       <c r="E20" s="12">
         <v>1.0</v>
       </c>
       <c r="F20" s="12">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="G20" s="12">
-        <v>64.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="H20" s="12">
+        <v>62.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -914,7 +962,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="12">
-        <v>130.0</v>
+        <v>115.0</v>
       </c>
       <c r="C21" s="12">
         <v>33.0</v>
@@ -926,262 +974,335 @@
         <v>1.0</v>
       </c>
       <c r="F21" s="12">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="G21" s="12">
-        <v>79.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="H21" s="12">
+        <v>64.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="B22" s="12">
+        <v>130.0</v>
+      </c>
+      <c r="C22" s="12">
+        <v>33.0</v>
+      </c>
+      <c r="D22" s="12">
+        <v>18.0</v>
+      </c>
+      <c r="E22" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="F22" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="H22" s="12">
+        <v>79.0</v>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="13"/>
+      <c r="A23" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="12">
+        <v>143.0</v>
+      </c>
+      <c r="C23" s="12">
+        <v>37.0</v>
+      </c>
+      <c r="D23" s="12">
+        <v>19.0</v>
+      </c>
+      <c r="E23" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="F23" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G23" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="H23" s="12">
+        <v>87.0</v>
+      </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="13"/>
+      <c r="A24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="13">
+        <v>154.0</v>
+      </c>
+      <c r="C24" s="13">
+        <v>40.0</v>
+      </c>
+      <c r="D24" s="13">
+        <v>19.0</v>
+      </c>
+      <c r="E24" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="F24" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="G24" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="H24" s="13">
+        <v>95.0</v>
+      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="13"/>
+      <c r="A25" s="14"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="13"/>
+      <c r="A26" s="14"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="13"/>
+      <c r="A27" s="14"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="13"/>
+      <c r="A28" s="14"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="13"/>
+      <c r="A29" s="14"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="13"/>
+      <c r="A30" s="14"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="13"/>
+      <c r="A31" s="14"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="13"/>
+      <c r="A32" s="14"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="13"/>
+      <c r="A33" s="14"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="13"/>
+      <c r="A34" s="14"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="13"/>
+      <c r="A35" s="14"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="13"/>
+      <c r="A36" s="14"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="13"/>
+      <c r="A37" s="14"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="13"/>
+      <c r="A38" s="14"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="13"/>
+      <c r="A39" s="14"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="13"/>
+      <c r="A40" s="14"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="13"/>
+      <c r="A41" s="14"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="13"/>
+      <c r="A42" s="14"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="13"/>
+      <c r="A43" s="14"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="13"/>
+      <c r="A44" s="14"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="13"/>
+      <c r="A45" s="14"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="13"/>
+      <c r="A46" s="14"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="13"/>
+      <c r="A47" s="14"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="13"/>
+      <c r="A48" s="14"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="13"/>
+      <c r="A49" s="14"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="13"/>
+      <c r="A50" s="14"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="13"/>
+      <c r="A51" s="14"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="13"/>
+      <c r="A52" s="14"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="13"/>
+      <c r="A53" s="14"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="13"/>
+      <c r="A54" s="14"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="13"/>
+      <c r="A55" s="14"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="13"/>
+      <c r="A56" s="14"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="13"/>
+      <c r="A57" s="14"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="13"/>
+      <c r="A58" s="14"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="13"/>
+      <c r="A59" s="14"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="13"/>
+      <c r="A60" s="14"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="13"/>
+      <c r="A61" s="14"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="13"/>
+      <c r="A62" s="14"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="13"/>
+      <c r="A63" s="14"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="13"/>
+      <c r="A64" s="14"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="13"/>
+      <c r="A65" s="14"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="13"/>
+      <c r="A66" s="14"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="13"/>
+      <c r="A67" s="14"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="13"/>
+      <c r="A68" s="14"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="13"/>
+      <c r="A69" s="14"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="13"/>
+      <c r="A70" s="14"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="13"/>
+      <c r="A71" s="14"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="13"/>
+      <c r="A72" s="14"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="13"/>
+      <c r="A73" s="14"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="13"/>
+      <c r="A74" s="14"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="13"/>
+      <c r="A75" s="14"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="13"/>
+      <c r="A76" s="14"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="13"/>
+      <c r="A77" s="14"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="13"/>
+      <c r="A78" s="14"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="13"/>
+      <c r="A79" s="14"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="13"/>
+      <c r="A80" s="14"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="13"/>
+      <c r="A81" s="14"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="13"/>
+      <c r="A82" s="14"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="13"/>
+      <c r="A83" s="14"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="13"/>
+      <c r="A84" s="14"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="13"/>
+      <c r="A85" s="14"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="13"/>
+      <c r="A86" s="14"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="13"/>
+      <c r="A87" s="14"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="13"/>
+      <c r="A88" s="14"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="13"/>
+      <c r="A89" s="14"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="13"/>
+      <c r="A90" s="14"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="13"/>
+      <c r="A91" s="14"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="13"/>
+      <c r="A92" s="14"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="13"/>
+      <c r="A93" s="14"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="13"/>
+      <c r="A94" s="14"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="13"/>
+      <c r="A95" s="14"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="13"/>
+      <c r="A96" s="14"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="13"/>
+      <c r="A97" s="14"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="13"/>
+      <c r="A98" s="14"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="13"/>
+      <c r="A99" s="14"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="13"/>
+      <c r="A100" s="14"/>
+    </row>
+    <row r="101" ht="15.75" customHeight="1">
+      <c r="A101" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A1:G1"/>
+  <mergeCells count="9">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Update March 29, 2020
</commit_message>
<xml_diff>
--- a/Daerah Istimewa Yogyakarta/01_DIY_Rekapitulasi_24032020.xlsx
+++ b/Daerah Istimewa Yogyakarta/01_DIY_Rekapitulasi_24032020.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>REKAPITULASI HARIAN KASUS COVID-19</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>28/3/2020</t>
+  </si>
+  <si>
+    <t>29/3/2020</t>
   </si>
 </sst>
 </file>
@@ -1039,30 +1042,53 @@
       <c r="A24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="12">
         <v>154.0</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="12">
         <v>40.0</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="12">
         <v>19.0</v>
       </c>
-      <c r="E24" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="F24" s="13">
+      <c r="E24" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="F24" s="12">
         <v>3.0</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="12">
         <v>4.0</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="12">
         <v>95.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="14"/>
+      <c r="A25" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="13">
+        <v>175.0</v>
+      </c>
+      <c r="C25" s="12">
+        <v>40.0</v>
+      </c>
+      <c r="D25" s="12">
+        <v>19.0</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="F25" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G25" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="H25" s="13">
+        <v>116.0</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="14"/>
@@ -1294,6 +1320,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="C3:C4"/>
@@ -1301,8 +1329,6 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>